<commit_message>
tidying up contact page
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 ContactPage.xlsx
+++ b/Testing Spreadsheet v1.0 ContactPage.xlsx
@@ -1573,7 +1573,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1659,7 +1659,6 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1735,6 +1734,7 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1742,11 +1742,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1754,11 +1757,14 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
+              <c:layout/>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1766,7 +1772,9 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                </c:ext>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -1813,7 +1821,7 @@
                   <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1836,6 +1844,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1905,7 +1914,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1926,11 +1935,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-731151744"/>
-        <c:axId val="-731151200"/>
+        <c:axId val="1921454096"/>
+        <c:axId val="1921454640"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-731151744"/>
+        <c:axId val="1921454096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1940,7 +1949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-731151200"/>
+        <c:crossAx val="1921454640"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1948,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-731151200"/>
+        <c:axId val="1921454640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1959,7 +1968,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-731151744"/>
+        <c:crossAx val="1921454096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2717,13 +2726,13 @@
       <c r="A19" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B19" s="35" t="s">
+      <c r="B19" s="34" t="s">
         <v>241</v>
       </c>
-      <c r="C19" s="35" t="s">
+      <c r="C19" s="34" t="s">
         <v>242</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2731,13 +2740,13 @@
       <c r="A20" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B20" s="35" t="s">
+      <c r="B20" s="34" t="s">
         <v>243</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="D20" s="35" t="s">
+      <c r="D20" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2745,13 +2754,13 @@
       <c r="A21" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="34" t="s">
         <v>245</v>
       </c>
-      <c r="C21" s="35" t="s">
+      <c r="C21" s="34" t="s">
         <v>244</v>
       </c>
-      <c r="D21" s="35" t="s">
+      <c r="D21" s="34" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2759,13 +2768,13 @@
       <c r="A22" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="34" t="s">
         <v>246</v>
       </c>
-      <c r="C22" s="35" t="s">
+      <c r="C22" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D22" s="35" t="s">
+      <c r="D22" s="34" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2773,13 +2782,13 @@
       <c r="A23" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="34" t="s">
         <v>247</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="34" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2787,13 +2796,13 @@
       <c r="A24" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="34" t="s">
         <v>248</v>
       </c>
-      <c r="C24" s="35" t="s">
+      <c r="C24" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="34" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2801,13 +2810,13 @@
       <c r="A25" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B25" s="35" t="s">
+      <c r="B25" s="34" t="s">
         <v>249</v>
       </c>
-      <c r="C25" s="35" t="s">
+      <c r="C25" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D25" s="35" t="s">
+      <c r="D25" s="34" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2815,13 +2824,13 @@
       <c r="A26" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="34" t="s">
         <v>250</v>
       </c>
-      <c r="C26" s="35" t="s">
+      <c r="C26" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="35" t="s">
+      <c r="D26" s="34" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2829,13 +2838,13 @@
       <c r="A27" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="34" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2843,13 +2852,13 @@
       <c r="A28" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B28" s="35" t="s">
+      <c r="B28" s="34" t="s">
         <v>252</v>
       </c>
-      <c r="C28" s="35" t="s">
+      <c r="C28" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D28" s="35" t="s">
+      <c r="D28" s="34" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2857,13 +2866,13 @@
       <c r="A29" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B29" s="35" t="s">
+      <c r="B29" s="34" t="s">
         <v>253</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D29" s="35" t="s">
+      <c r="D29" s="34" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2871,13 +2880,13 @@
       <c r="A30" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="35" t="s">
+      <c r="D30" s="34" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2925,8 +2934,8 @@
   </sheetPr>
   <dimension ref="A1:Z160"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3047,7 +3056,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="99.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="114" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>79</v>
       </c>
@@ -3072,7 +3081,7 @@
       <c r="H3" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="33" t="s">
+      <c r="I3" s="35" t="s">
         <v>66</v>
       </c>
       <c r="J3" s="3" t="s">
@@ -3123,7 +3132,7 @@
       <c r="H4" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="33" t="s">
+      <c r="I4" s="35" t="s">
         <v>66</v>
       </c>
       <c r="J4" s="3" t="s">
@@ -3174,7 +3183,7 @@
       <c r="H5" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="35" t="s">
         <v>66</v>
       </c>
       <c r="J5" s="3" t="s">
@@ -3390,8 +3399,8 @@
         <v>25</v>
       </c>
       <c r="U9" s="31">
-        <f>COUNTIF(H3:H89,"*Failed*")</f>
-        <v>9</v>
+        <f>COUNTIF(H2:H89,"*Failed*")</f>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="42.75" x14ac:dyDescent="0.25">
@@ -3433,7 +3442,7 @@
         <v>54</v>
       </c>
       <c r="U10" s="31">
-        <f>COUNTIF(H4:H89,"*Not*")</f>
+        <f>COUNTIF(H2:H89,"*Not*")</f>
         <v>0</v>
       </c>
     </row>
@@ -3938,7 +3947,7 @@
       <c r="L24" s="4"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
-      <c r="O24" s="36"/>
+      <c r="O24" s="35"/>
       <c r="P24" s="9"/>
     </row>
     <row r="25" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
@@ -3969,12 +3978,12 @@
       <c r="I25" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="J25" s="36"/>
+      <c r="J25" s="35"/>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
-      <c r="M25" s="36"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="36"/>
+      <c r="M25" s="35"/>
+      <c r="N25" s="35"/>
+      <c r="O25" s="35"/>
       <c r="P25" s="9"/>
       <c r="T25" t="s">
         <v>56</v>
@@ -4008,12 +4017,12 @@
       <c r="I26" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="J26" s="36"/>
+      <c r="J26" s="35"/>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="36"/>
-      <c r="O26" s="36"/>
+      <c r="M26" s="35"/>
+      <c r="N26" s="35"/>
+      <c r="O26" s="35"/>
       <c r="P26" s="9"/>
       <c r="T26" t="s">
         <v>34</v>
@@ -4051,19 +4060,19 @@
       <c r="I27" s="13" t="s">
         <v>269</v>
       </c>
-      <c r="J27" s="36"/>
+      <c r="J27" s="35"/>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
-      <c r="M27" s="36"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="36"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
       <c r="P27" s="9"/>
       <c r="T27" t="s">
         <v>57</v>
       </c>
       <c r="U27" s="31">
-        <f>COUNTIF(L2:L7,"*Moderate*")</f>
-        <v>5</v>
+        <f>COUNTIF(L2:L49,"*Moderate*")</f>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
@@ -4105,7 +4114,7 @@
         <v>35</v>
       </c>
       <c r="U28" s="31">
-        <f>COUNTIF(L2:L7,"*Major*")</f>
+        <f>COUNTIF(L2:L49,"*Major*")</f>
         <v>1</v>
       </c>
     </row>
@@ -4141,12 +4150,12 @@
         <v>303</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L29" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M29" s="37">
+      <c r="M29" s="36">
         <v>42108</v>
       </c>
       <c r="N29" s="9"/>
@@ -4158,7 +4167,7 @@
         <v>36</v>
       </c>
       <c r="U29" s="31">
-        <f>COUNTIF(L2:L7,"*Critical*")</f>
+        <f>COUNTIF(L2:L49,"*Critical*")</f>
         <v>0</v>
       </c>
     </row>
@@ -4229,7 +4238,7 @@
       <c r="J31" s="9"/>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
-      <c r="M31" s="37"/>
+      <c r="M31" s="36"/>
       <c r="N31" s="9"/>
       <c r="O31" s="1"/>
       <c r="P31" s="9"/>
@@ -4302,12 +4311,12 @@
         <v>304</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M33" s="37">
+      <c r="M33" s="36">
         <v>42108</v>
       </c>
       <c r="N33" s="9"/>
@@ -4420,12 +4429,12 @@
         <v>305</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L36" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="M36" s="37">
+      <c r="M36" s="36">
         <v>42108</v>
       </c>
       <c r="N36" s="9"/>
@@ -4438,7 +4447,7 @@
       <c r="A37" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="37" t="s">
         <v>288</v>
       </c>
       <c r="C37" s="1" t="s">
@@ -6227,7 +6236,7 @@
           <x14:formula1>
             <xm:f>Settings!$D$4:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K11</xm:sqref>
+          <xm:sqref>K2:K11 K29 K33 K36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -6239,7 +6248,7 @@
           <x14:formula1>
             <xm:f>[3]Settings!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>K33 K36 K24:K31</xm:sqref>
+          <xm:sqref>K30:K31 K24:K28</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
@@ -6537,7 +6546,7 @@
       <c r="D11" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="E11" s="33" t="s">
         <v>201</v>
       </c>
       <c r="F11" s="1"/>
@@ -7114,12 +7123,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -7233,6 +7236,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
   <ds:schemaRefs>
@@ -7242,15 +7251,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{64745CD4-DB27-427B-80D9-1CCB91D6E4BC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7264,4 +7264,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to Contact Page
</commit_message>
<xml_diff>
--- a/Testing Spreadsheet v1.0 ContactPage.xlsx
+++ b/Testing Spreadsheet v1.0 ContactPage.xlsx
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_Toc407532261" localSheetId="0">Reqs!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -1911,10 +1911,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -1935,11 +1935,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="1921454096"/>
-        <c:axId val="1921454640"/>
+        <c:axId val="125923392"/>
+        <c:axId val="125924480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1921454096"/>
+        <c:axId val="125923392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1949,7 +1949,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1921454640"/>
+        <c:crossAx val="125924480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1957,7 +1957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1921454640"/>
+        <c:axId val="125924480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1968,7 +1968,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="1921454096"/>
+        <c:crossAx val="125923392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2934,8 +2934,8 @@
   </sheetPr>
   <dimension ref="A1:Z160"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="C25" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="U26" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3091,7 +3091,7 @@
         <v>31</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M3" s="32">
         <v>42108</v>
@@ -3142,7 +3142,7 @@
         <v>31</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M4" s="32">
         <v>42108</v>
@@ -3193,7 +3193,7 @@
         <v>31</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M5" s="32">
         <v>42108</v>
@@ -3206,7 +3206,7 @@
       </c>
       <c r="P5" s="9"/>
     </row>
-    <row r="6" spans="1:26" ht="85.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="71.25" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>98</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>31</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M6" s="32">
         <v>42108</v>
@@ -3289,7 +3289,7 @@
         <v>31</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M7" s="32">
         <v>42108</v>
@@ -3340,7 +3340,7 @@
         <v>31</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="M8" s="32">
         <v>42108</v>
@@ -4029,7 +4029,7 @@
       </c>
       <c r="U26" s="31">
         <f>COUNTIF(L2:L49,"*Minor*")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
@@ -4072,7 +4072,7 @@
       </c>
       <c r="U27" s="31">
         <f>COUNTIF(L2:L49,"*Moderate*")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:21" ht="99.75" x14ac:dyDescent="0.25">
@@ -7114,12 +7114,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7237,15 +7234,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7267,10 +7268,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEF49AB9-68C3-4E70-84F5-930D4AF0373D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A346E62E-1A2C-4E03-B91F-FE4FC47F8E89}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>